<commit_message>
added a sample invoice
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DocsShare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B6DC1A-F712-4200-811D-32DB3454F2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060A646F-F7AC-44DD-A3B7-DEF3372B2118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11020" xr2:uid="{80206310-6E0A-4238-B6F7-FA0DBB82C50D}"/>
   </bookViews>
@@ -97,6 +97,9 @@
     </r>
   </si>
   <si>
+    <t>Development of Intranet Site and IT Helpdesk using updated technologies. Edit and update options in FA services and Inventory Management(leftover).</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -116,7 +119,49 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: Created pages for editing the erroneous data or updating to new values shared by desktop engineers(Update Modules developed : System Location, Make and Model, OS updates, Office Software availability and version changes, Hostname and Serial Number). Created search modules for Activating/De-activating users, application admins, systems at different locations, services.
+      <t xml:space="preserve">: Created pages for editing the erroneous data or updating to new values shared by desktop engineers(Update Modules developed : System Location, Make and Model, OS updates, Office Software availability and version changes, Hostname and Serial Number). Created search modules for Activating/De-activating users, application admins, systems at different locations, services. Developed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>QR-Code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BarCode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for each and every system, hardware. On scanning the QR-Code, the details of the system, along with system history(any previous assignment of system, any changes in software or hardware, maintenance activity will be shown in a password protected PDF. Only IT personnel have access to open).
 </t>
     </r>
     <r>
@@ -140,9 +185,6 @@
       </rPr>
       <t xml:space="preserve"> Modules created : Update modules and search modules. Updating or correcting existing data(if any mistakes present), search modules for different types of visitors and staff, location wise, month, day, year and overall data wise. Edit option for visitors, honoured guest and staff were given to Facility and Security personnel based on the location and registration(VLS or VLL).</t>
     </r>
-  </si>
-  <si>
-    <t>Development of Intranet Site and IT Helpdesk using updated technologies. Edit and update options in FA services and Inventory Management(leftover).</t>
   </si>
 </sst>
 </file>
@@ -233,13 +275,15 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -247,8 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -569,7 +611,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,63 +627,63 @@
       <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
+      <c r="A3" s="4">
         <v>45383</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
+      <c r="A4" s="4">
         <v>45413</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>45444</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <v>45474</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>45505</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="191" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>45536</v>
+      </c>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="149.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
-        <v>45536</v>
-      </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>